<commit_message>
alteracoes finais e documentacao pdf
</commit_message>
<xml_diff>
--- a/src/main/java/com/mycompany/n2_prog3_mateusalmeida/dados/DadosClinicaHospitalar.xlsx
+++ b/src/main/java/com/mycompany/n2_prog3_mateusalmeida/dados/DadosClinicaHospitalar.xlsx
@@ -117,10 +117,10 @@
     <t>id Responsavel</t>
   </si>
   <si>
-    <t>Teste Paciente 1</t>
-  </si>
-  <si>
-    <t>21/01/2009</t>
+    <t>Teste Paciente Exec</t>
+  </si>
+  <si>
+    <t>20/01/2009</t>
   </si>
   <si>
     <t>F</t>

</xml_diff>